<commit_message>
Clean up project structure and add network support - Remove unnecessary files - Update server port to 3002 to avoid conflicts - Add network-ready configuration - Update API endpoints for network access - Add requirements.txt for Python dependencies - Update README.md with comprehensive documentation - Add start-network.bat for easy startup
</commit_message>
<xml_diff>
--- a/process/outputs/excel_files/APInvoicesImport1.xlsx
+++ b/process/outputs/excel_files/APInvoicesImport1.xlsx
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>07/07/25</t>
+          <t>08/04/25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2209,11 +2209,13 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SSFLUM</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>106271</v>
+          <t>LORSON</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>01-871062</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -2222,11 +2224,11 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>07/07/25</t>
+          <t>08/04/25</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>138.24</v>
+        <v>89</v>
       </c>
       <c r="R2" t="inlineStr"/>
       <c r="T2" t="n">
@@ -2234,7 +2236,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>25.16</t>
+          <t>25.09</t>
         </is>
       </c>
       <c r="V2" t="n">

</xml_diff>

<commit_message>
Fix vendor approval dialog and processing flow - Fixed TypeError in vendor-approval-dialog.tsx - Fixed React Hooks order violation - Improved CSV parsing in backend for vendor matches - Added content hash tracking to prevent showing old data - Enhanced approval dialog UI with single row layout - Fixed processing animation timing and z-index issues - Added post-approval processing animation - Implemented raw_pdfs folder monitoring for completion - Added comprehensive debugging and error handling
</commit_message>
<xml_diff>
--- a/process/outputs/excel_files/APInvoicesImport1.xlsx
+++ b/process/outputs/excel_files/APInvoicesImport1.xlsx
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>08/04/25</t>
+          <t>08/06/25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2209,12 +2209,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>LORSON</t>
+          <t>JONSUP</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>01-871062</t>
+          <t>110-S10112669.001</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -2224,33 +2224,29 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>08/04/25</t>
+          <t>08/06/25</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>89</v>
-      </c>
-      <c r="R2" t="inlineStr"/>
+        <v>99.31</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>San Leandro Unit Install</t>
+        </is>
+      </c>
       <c r="T2" t="n">
-        <v>5030</v>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>25.09</t>
-        </is>
-      </c>
-      <c r="V2" t="n">
-        <v>320</v>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr"/>
+        <v>5260</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>!Material</t>
+          <t>!Service Material</t>
         </is>
       </c>
       <c r="BE2" t="inlineStr">

</xml_diff>

<commit_message>
Implement vendor and PO approval dialogs with robust timing and data validation
</commit_message>
<xml_diff>
--- a/process/outputs/excel_files/APInvoicesImport1.xlsx
+++ b/process/outputs/excel_files/APInvoicesImport1.xlsx
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>08/06/25</t>
+          <t>07/28/25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2209,13 +2209,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>JONSUP</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>110-S10112669.001</t>
-        </is>
+          <t>SLABRO</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>860166732</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -2224,31 +2222,22 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>08/06/25</t>
+          <t>07/28/25</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>99.31</v>
+        <v>81.53</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>San Leandro Unit Install</t>
+          <t>Shop</t>
         </is>
       </c>
       <c r="T2" t="n">
-        <v>5260</v>
+        <v>1200</v>
       </c>
       <c r="U2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>!Service Material</t>
-        </is>
-      </c>
+      <c r="AA2" t="inlineStr"/>
       <c r="BE2" t="inlineStr">
         <is>
           <t>1000</t>

</xml_diff>

<commit_message>
Remove Processing Complete notification and update approval dialogs - Removed the green Processing Complete notification card from the dashboard - Updated vendor and PO approval dialogs with improved functionality - Enhanced file name display to prevent overlap - Added uploads folder check for empty state - Improved processing flow and user experience
</commit_message>
<xml_diff>
--- a/process/outputs/excel_files/APInvoicesImport1.xlsx
+++ b/process/outputs/excel_files/APInvoicesImport1.xlsx
@@ -1847,7 +1847,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF2"/>
+  <dimension ref="A1:BF19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
@@ -2199,51 +2199,1237 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>07/07/25</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>SSFLUM</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>106271</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>07/07/25</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>138.24</v>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="T2" t="n">
+        <v>5030</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>25.16</t>
+        </is>
+      </c>
+      <c r="V2" t="n">
+        <v>320</v>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>!Material</t>
+        </is>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>SSFLUM</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>106386</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>4.81</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
+      <c r="T3" t="n">
+        <v>5030</v>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>25.02</t>
+        </is>
+      </c>
+      <c r="V3" t="n">
+        <v>320</v>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>!Material</t>
+        </is>
+      </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>07/15/25</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>SSFLUM</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>106465</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>07/15/25</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>36.7</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>PO # SHOP</t>
+        </is>
+      </c>
+      <c r="T4" t="n">
+        <v>5260</v>
+      </c>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>!Service Material</t>
+        </is>
+      </c>
+      <c r="BE4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>07/22/25</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>SSFLUM</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>106699</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>07/22/25</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>6.91</v>
+      </c>
+      <c r="R5" t="inlineStr"/>
+      <c r="T5" t="n">
+        <v>5030</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>25.27</t>
+        </is>
+      </c>
+      <c r="V5" t="n">
+        <v>320</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>!Material</t>
+        </is>
+      </c>
+      <c r="BE5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>07/22/25</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>SSFLUM</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>106700</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>07/22/25</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>6.91</v>
+      </c>
+      <c r="R6" t="inlineStr"/>
+      <c r="T6" t="n">
+        <v>5030</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>25.02</t>
+        </is>
+      </c>
+      <c r="V6" t="n">
+        <v>320</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>!Material</t>
+        </is>
+      </c>
+      <c r="BE6" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF6" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>07/28/25</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>testraj</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>SSFLUM</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>107155</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>07/28/25</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>36.3</v>
+      </c>
+      <c r="R7" t="inlineStr"/>
+      <c r="T7" t="n">
+        <v>5030</v>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>25.04</t>
+        </is>
+      </c>
+      <c r="V7" t="n">
+        <v>320</v>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>!Material</t>
+        </is>
+      </c>
+      <c r="BE7" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF7" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>07/30/25</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>SSFLUM</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>107274</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>07/30/25</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>33.06</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>650-615-0248</t>
+        </is>
+      </c>
+      <c r="T8" t="n">
+        <v>5260</v>
+      </c>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>!Service Material</t>
+        </is>
+      </c>
+      <c r="BE8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>07/28/25</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>SLABRO</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>860166732</v>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>860166732</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>07/28/25</t>
         </is>
       </c>
-      <c r="J2" t="n">
+      <c r="J9" t="n">
         <v>81.53</v>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>Shop</t>
         </is>
       </c>
-      <c r="T2" t="n">
+      <c r="T9" t="n">
         <v>1200</v>
       </c>
-      <c r="U2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="BE2" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF2" t="inlineStr">
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="BE9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>07/30/25</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>SLABRO</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>860186777</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>07/30/25</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>1791.43</v>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>SHOP</t>
+        </is>
+      </c>
+      <c r="T10" t="n">
+        <v>1200</v>
+      </c>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="BE10" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF10" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>07/30/25</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>SLABRO</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>860184845</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>07/30/25</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>190.16</v>
+      </c>
+      <c r="R11" t="inlineStr"/>
+      <c r="T11" t="n">
+        <v>5030</v>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>25.28</t>
+        </is>
+      </c>
+      <c r="V11" t="n">
+        <v>320</v>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>!Material</t>
+        </is>
+      </c>
+      <c r="BE11" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF11" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>AIRSUP</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>IN1019091</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>41.7</v>
+      </c>
+      <c r="R12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="BE12" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF12" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LORSON</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>01-871043</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>104.38</v>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>SHOP STOCK</t>
+        </is>
+      </c>
+      <c r="T13" t="n">
+        <v>1200</v>
+      </c>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="BE13" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF13" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LORSON</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>01-871062</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>89</v>
+      </c>
+      <c r="R14" t="inlineStr"/>
+      <c r="T14" t="n">
+        <v>5030</v>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>25.09</t>
+        </is>
+      </c>
+      <c r="V14" t="n">
+        <v>320</v>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>!Material</t>
+        </is>
+      </c>
+      <c r="BE14" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF14" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LORSON</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>01-871060</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>356</v>
+      </c>
+      <c r="R15" t="inlineStr"/>
+      <c r="T15" t="n">
+        <v>5030</v>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>25.09</t>
+        </is>
+      </c>
+      <c r="V15" t="n">
+        <v>320</v>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>!Material</t>
+        </is>
+      </c>
+      <c r="BE15" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF15" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>JONSUP</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>110-S101125942.001</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>107.3</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Ricky's Truck Stock</t>
+        </is>
+      </c>
+      <c r="T16" t="n">
+        <v>5260</v>
+      </c>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>!Service Material</t>
+        </is>
+      </c>
+      <c r="BE16" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF16" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>OMNDUC</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1179219</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>734.34</v>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>950</t>
+        </is>
+      </c>
+      <c r="T17" t="n">
+        <v>5260</v>
+      </c>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>!Service Material</t>
+        </is>
+      </c>
+      <c r="BE17" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF17" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>OMNDUC</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1179217</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>08/04/25</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>1122.48</v>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>HOME 2 SUITES</t>
+        </is>
+      </c>
+      <c r="T18" t="n">
+        <v>5260</v>
+      </c>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>!Service Material</t>
+        </is>
+      </c>
+      <c r="BE18" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF18" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>08/05/25</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>testraj</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>OMNDUC</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1179211</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>08/05/25</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>11875.42</v>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>TOKYO</t>
+        </is>
+      </c>
+      <c r="T19" t="n">
+        <v>5260</v>
+      </c>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>!Service Material</t>
+        </is>
+      </c>
+      <c r="BE19" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF19" t="inlineStr">
         <is>
           <t>1000</t>
         </is>

</xml_diff>

<commit_message>
Fix approval dialogs and data persistence issues - Prevent dialogs from closing on outside click - Add warning banners and clear instructions - Ensure edited PO data is saved to pixtral_po_results.csv - Update server.js to handle PO approval data updates - Modify Python script to re-read updated CSV data after approval - Fix React hooks order issues in vendor approval dialog - Add comprehensive error handling and null checks
</commit_message>
<xml_diff>
--- a/process/outputs/excel_files/APInvoicesImport1.xlsx
+++ b/process/outputs/excel_files/APInvoicesImport1.xlsx
@@ -1847,7 +1847,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF19"/>
+  <dimension ref="A1:BF3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>07/07/25</t>
+          <t>08/06/25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2209,12 +2209,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SSFLUM</t>
+          <t>LORSON</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>106271</t>
+          <t>01-871775</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -2224,11 +2224,11 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>07/07/25</t>
+          <t>08/06/25</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>138.24</v>
+        <v>453.05</v>
       </c>
       <c r="R2" t="inlineStr"/>
       <c r="T2" t="n">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>25.16</t>
+          <t>25.04</t>
         </is>
       </c>
       <c r="V2" t="n">
@@ -2270,7 +2270,11 @@
           <t>TST</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>08/06/25</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>testraj</t>
@@ -2278,12 +2282,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>SSFLUM</t>
+          <t>JONSUP</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>106386</t>
+          <t>110-S10112669.001</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -2291,31 +2295,33 @@
           <t>I</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>08/06/25</t>
+        </is>
+      </c>
       <c r="J3" t="n">
-        <v>4.81</v>
-      </c>
-      <c r="R3" t="inlineStr"/>
+        <v>99.31</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>San Leandro Unit Install</t>
+        </is>
+      </c>
       <c r="T3" t="n">
-        <v>5030</v>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>25.02</t>
-        </is>
-      </c>
-      <c r="V3" t="n">
-        <v>320</v>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr"/>
+        <v>5260</v>
+      </c>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>!Material</t>
+          <t>!Service Material</t>
         </is>
       </c>
       <c r="BE3" t="inlineStr">
@@ -2324,1112 +2330,6 @@
         </is>
       </c>
       <c r="BF3" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>07/15/25</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>SSFLUM</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>106465</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>07/15/25</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>PO # SHOP</t>
-        </is>
-      </c>
-      <c r="T4" t="n">
-        <v>5260</v>
-      </c>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>!Service Material</t>
-        </is>
-      </c>
-      <c r="BE4" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF4" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>07/22/25</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>SSFLUM</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>106699</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>07/22/25</t>
-        </is>
-      </c>
-      <c r="J5" t="n">
-        <v>6.91</v>
-      </c>
-      <c r="R5" t="inlineStr"/>
-      <c r="T5" t="n">
-        <v>5030</v>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>25.27</t>
-        </is>
-      </c>
-      <c r="V5" t="n">
-        <v>320</v>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr"/>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>!Material</t>
-        </is>
-      </c>
-      <c r="BE5" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF5" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>07/22/25</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>SSFLUM</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>106700</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>07/22/25</t>
-        </is>
-      </c>
-      <c r="J6" t="n">
-        <v>6.91</v>
-      </c>
-      <c r="R6" t="inlineStr"/>
-      <c r="T6" t="n">
-        <v>5030</v>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>25.02</t>
-        </is>
-      </c>
-      <c r="V6" t="n">
-        <v>320</v>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>!Material</t>
-        </is>
-      </c>
-      <c r="BE6" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF6" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>07/28/25</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>SSFLUM</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>107155</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>07/28/25</t>
-        </is>
-      </c>
-      <c r="J7" t="n">
-        <v>36.3</v>
-      </c>
-      <c r="R7" t="inlineStr"/>
-      <c r="T7" t="n">
-        <v>5030</v>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>25.04</t>
-        </is>
-      </c>
-      <c r="V7" t="n">
-        <v>320</v>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>!Material</t>
-        </is>
-      </c>
-      <c r="BE7" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF7" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>07/30/25</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>SSFLUM</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>107274</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>07/30/25</t>
-        </is>
-      </c>
-      <c r="J8" t="n">
-        <v>33.06</v>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>650-615-0248</t>
-        </is>
-      </c>
-      <c r="T8" t="n">
-        <v>5260</v>
-      </c>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>!Service Material</t>
-        </is>
-      </c>
-      <c r="BE8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>07/28/25</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>SLABRO</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>860166732</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>07/28/25</t>
-        </is>
-      </c>
-      <c r="J9" t="n">
-        <v>81.53</v>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>Shop</t>
-        </is>
-      </c>
-      <c r="T9" t="n">
-        <v>1200</v>
-      </c>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
-      <c r="BE9" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF9" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>07/30/25</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>SLABRO</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>860186777</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>07/30/25</t>
-        </is>
-      </c>
-      <c r="J10" t="n">
-        <v>1791.43</v>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>SHOP</t>
-        </is>
-      </c>
-      <c r="T10" t="n">
-        <v>1200</v>
-      </c>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
-      <c r="BE10" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF10" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>07/30/25</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>SLABRO</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>860184845</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>07/30/25</t>
-        </is>
-      </c>
-      <c r="J11" t="n">
-        <v>190.16</v>
-      </c>
-      <c r="R11" t="inlineStr"/>
-      <c r="T11" t="n">
-        <v>5030</v>
-      </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>25.28</t>
-        </is>
-      </c>
-      <c r="V11" t="n">
-        <v>320</v>
-      </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="AA11" t="inlineStr"/>
-      <c r="AB11" t="inlineStr">
-        <is>
-          <t>!Material</t>
-        </is>
-      </c>
-      <c r="BE11" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF11" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>AIRSUP</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>IN1019091</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="J12" t="n">
-        <v>41.7</v>
-      </c>
-      <c r="R12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
-      <c r="AA12" t="inlineStr"/>
-      <c r="BE12" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF12" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>LORSON</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>01-871043</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="J13" t="n">
-        <v>104.38</v>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>SHOP STOCK</t>
-        </is>
-      </c>
-      <c r="T13" t="n">
-        <v>1200</v>
-      </c>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
-      <c r="BE13" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF13" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>LORSON</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>01-871062</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="J14" t="n">
-        <v>89</v>
-      </c>
-      <c r="R14" t="inlineStr"/>
-      <c r="T14" t="n">
-        <v>5030</v>
-      </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>25.09</t>
-        </is>
-      </c>
-      <c r="V14" t="n">
-        <v>320</v>
-      </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="inlineStr">
-        <is>
-          <t>!Material</t>
-        </is>
-      </c>
-      <c r="BE14" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF14" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>LORSON</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>01-871060</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="J15" t="n">
-        <v>356</v>
-      </c>
-      <c r="R15" t="inlineStr"/>
-      <c r="T15" t="n">
-        <v>5030</v>
-      </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>25.09</t>
-        </is>
-      </c>
-      <c r="V15" t="n">
-        <v>320</v>
-      </c>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr">
-        <is>
-          <t>!Material</t>
-        </is>
-      </c>
-      <c r="BE15" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF15" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>JONSUP</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>110-S101125942.001</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="J16" t="n">
-        <v>107.3</v>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>Ricky's Truck Stock</t>
-        </is>
-      </c>
-      <c r="T16" t="n">
-        <v>5260</v>
-      </c>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="AB16" t="inlineStr">
-        <is>
-          <t>!Service Material</t>
-        </is>
-      </c>
-      <c r="BE16" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF16" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>OMNDUC</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>1179219</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="J17" t="n">
-        <v>734.34</v>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>950</t>
-        </is>
-      </c>
-      <c r="T17" t="n">
-        <v>5260</v>
-      </c>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr"/>
-      <c r="AA17" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="AB17" t="inlineStr">
-        <is>
-          <t>!Service Material</t>
-        </is>
-      </c>
-      <c r="BE17" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF17" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>OMNDUC</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>1179217</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="J18" t="n">
-        <v>1122.48</v>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>HOME 2 SUITES</t>
-        </is>
-      </c>
-      <c r="T18" t="n">
-        <v>5260</v>
-      </c>
-      <c r="U18" t="inlineStr"/>
-      <c r="V18" t="inlineStr"/>
-      <c r="W18" t="inlineStr"/>
-      <c r="AA18" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="AB18" t="inlineStr">
-        <is>
-          <t>!Service Material</t>
-        </is>
-      </c>
-      <c r="BE18" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF18" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>08/05/25</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>OMNDUC</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>1179211</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>08/05/25</t>
-        </is>
-      </c>
-      <c r="J19" t="n">
-        <v>11875.42</v>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>TOKYO</t>
-        </is>
-      </c>
-      <c r="T19" t="n">
-        <v>5260</v>
-      </c>
-      <c r="U19" t="inlineStr"/>
-      <c r="V19" t="inlineStr"/>
-      <c r="W19" t="inlineStr"/>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="AB19" t="inlineStr">
-        <is>
-          <t>!Service Material</t>
-        </is>
-      </c>
-      <c r="BE19" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF19" t="inlineStr">
         <is>
           <t>1000</t>
         </is>

</xml_diff>

<commit_message>
Fix light theme styling and processing animation - Revert light theme colors to original values - Fix processing animation to use theme-aware colors - Improve approval dialog button styling for light theme - Remove hardcoded green colors from Approve All buttons - Use theme-aware colors for better consistency - Add subtle shadows and hover effects - Maintain original light theme appearance while improving usability
</commit_message>
<xml_diff>
--- a/process/outputs/excel_files/APInvoicesImport1.xlsx
+++ b/process/outputs/excel_files/APInvoicesImport1.xlsx
@@ -1847,7 +1847,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF3"/>
+  <dimension ref="A1:BF2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>08/06/25</t>
+          <t>08/04/25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2209,12 +2209,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>LORSON</t>
+          <t>JONSUP</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>01-871775</t>
+          <t>110-S101125942.001</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -2224,33 +2224,29 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>08/06/25</t>
+          <t>08/04/25</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>453.05</v>
-      </c>
-      <c r="R2" t="inlineStr"/>
+        <v>107.3</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Ricky's Truck Stock</t>
+        </is>
+      </c>
       <c r="T2" t="n">
-        <v>5030</v>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>25.04</t>
-        </is>
-      </c>
-      <c r="V2" t="n">
-        <v>320</v>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr"/>
+        <v>5260</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>!Material</t>
+          <t>!Service Material</t>
         </is>
       </c>
       <c r="BE2" t="inlineStr">
@@ -2259,77 +2255,6 @@
         </is>
       </c>
       <c r="BF2" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>08/06/25</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>JONSUP</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>110-S10112669.001</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>08/06/25</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
-        <v>99.31</v>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>San Leandro Unit Install</t>
-        </is>
-      </c>
-      <c r="T3" t="n">
-        <v>5260</v>
-      </c>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>!Service Material</t>
-        </is>
-      </c>
-      <c r="BE3" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF3" t="inlineStr">
         <is>
           <t>1000</t>
         </is>

</xml_diff>

<commit_message>
Add file deletion functionality and refactor uploaded files display to modal dialog
</commit_message>
<xml_diff>
--- a/process/outputs/excel_files/APInvoicesImport1.xlsx
+++ b/process/outputs/excel_files/APInvoicesImport1.xlsx
@@ -1847,7 +1847,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF2"/>
+  <dimension ref="A1:BF1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
@@ -2191,75 +2191,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>TST</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>testraj</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>JONSUP</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>110-S101125942.001</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>08/04/25</t>
-        </is>
-      </c>
-      <c r="J2" t="n">
-        <v>107.3</v>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Ricky's Truck Stock</t>
-        </is>
-      </c>
-      <c r="T2" t="n">
-        <v>5260</v>
-      </c>
-      <c r="U2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>!Service Material</t>
-        </is>
-      </c>
-      <c r="BE2" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="BF2" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Update invoice parser with enhanced UI components, pipeline improvements, and new documentation
</commit_message>
<xml_diff>
--- a/process/outputs/excel_files/APInvoicesImport1.xlsx
+++ b/process/outputs/excel_files/APInvoicesImport1.xlsx
@@ -1847,7 +1847,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF1"/>
+  <dimension ref="A1:BF6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
@@ -2191,6 +2191,361 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AA1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>02/05/25</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>AIRTEC</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>176048</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>02/05/25</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>87.90000000000001</v>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="T2" t="n">
+        <v>5040</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>23.30</t>
+        </is>
+      </c>
+      <c r="V2" t="n">
+        <v>330</v>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>!Equipment</t>
+        </is>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AA1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>02/05/25</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>AIRTEC</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>176049</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>02/05/25</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>532.89</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
+      <c r="T3" t="n">
+        <v>5040</v>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>21.45</t>
+        </is>
+      </c>
+      <c r="V3" t="n">
+        <v>330</v>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>!Equipment</t>
+        </is>
+      </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AA1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>02/14/25</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>AIRTEC</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>176087</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>02/14/25</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>49.44</v>
+      </c>
+      <c r="R4" t="inlineStr"/>
+      <c r="T4" t="n">
+        <v>5040</v>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>23.30</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
+        <v>330</v>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>!Equipment</t>
+        </is>
+      </c>
+      <c r="BE4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AA1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>02/19/25</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>AIRTEC</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>176106</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>02/19/25</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>3098.48</v>
+      </c>
+      <c r="R5" t="inlineStr"/>
+      <c r="T5" t="n">
+        <v>5040</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>24.46</t>
+        </is>
+      </c>
+      <c r="V5" t="n">
+        <v>330</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>!Equipment</t>
+        </is>
+      </c>
+      <c r="BE5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AA1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>02/19/25</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>AIRTEC</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>176107</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>02/19/25</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>208.76</v>
+      </c>
+      <c r="R6" t="inlineStr"/>
+      <c r="T6" t="n">
+        <v>5040</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>24.46</t>
+        </is>
+      </c>
+      <c r="V6" t="n">
+        <v>330</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>!Equipment</t>
+        </is>
+      </c>
+      <c r="BE6" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="BF6" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>